<commit_message>
moved files to make public
</commit_message>
<xml_diff>
--- a/docs/MME paper tables, initial submission.xlsx
+++ b/docs/MME paper tables, initial submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nabarun/Documents/GitHub/MMEequations/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E316CC0-85D3-074F-A3F5-8132330A214E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218DA06B-B5C9-354B-A000-A07F2E0828E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18000" yWindow="760" windowWidth="31960" windowHeight="20820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4900" yWindow="5300" windowWidth="31960" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 1 data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Table 2 meta analysis" sheetId="8" r:id="rId3"/>
     <sheet name="Table 3 sensitivity" sheetId="5" r:id="rId4"/>
     <sheet name="Table 4 recommendations" sheetId="7" r:id="rId5"/>
-    <sheet name="Cut-points test" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="141">
   <si>
     <t>Daily MME Definition</t>
   </si>
@@ -179,57 +178,6 @@
   </si>
   <si>
     <t>Median of Daily MME (IQR)</t>
-  </si>
-  <si>
-    <t>With &gt;50, &gt;90, &gt;120 daily MME</t>
-  </si>
-  <si>
-    <t>Daily MME &gt;50</t>
-  </si>
-  <si>
-    <t>Daily MME &gt;90</t>
-  </si>
-  <si>
-    <t>Daily MME &gt;120</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># of Patient </t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>pat_mme1</t>
-  </si>
-  <si>
-    <t>pat_mme2</t>
-  </si>
-  <si>
-    <t>pat_mme3</t>
-  </si>
-  <si>
-    <t>pat_mme4</t>
-  </si>
-  <si>
-    <t>pat_mme5</t>
-  </si>
-  <si>
-    <t>Daily MME ≥50</t>
-  </si>
-  <si>
-    <t>Daily MME ≥90</t>
-  </si>
-  <si>
-    <t>Daily MME ≥120</t>
-  </si>
-  <si>
-    <t>With ≥50, ≥90, ≥120 daily MME</t>
-  </si>
-  <si>
-    <t>Percent increase</t>
-  </si>
-  <si>
-    <t>Absolute increase</t>
   </si>
   <si>
     <t>All opioid patients</t>
@@ -818,10 +766,6 @@
     <t>Table 2. Meta analysis comparing Florida and California, by daily MME definition variant</t>
   </si>
   <si>
-    <t>Difference in Mean of Daily MME
-(95% CI)</t>
-  </si>
-  <si>
     <t>Percent more "High Dose" Patients 
 (95% CI)</t>
   </si>
@@ -833,16 +777,20 @@
   </si>
   <si>
     <t>Table 1. Average and median daily MME by type of pain medication in Florida and California, by daily MME variant</t>
+  </si>
+  <si>
+    <t>Milligram Difference
+in Mean Daily MME
+(95% CI)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
   <fonts count="13">
@@ -935,18 +883,12 @@
       <name val="Calibri (Body)"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -1016,15 +958,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1077,49 +1018,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="5" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1178,12 +1076,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1285,12 +1177,11 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1622,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:G20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1634,7 +1525,7 @@
   <sheetData>
     <row r="4" spans="3:7">
       <c r="C4" s="3" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -1643,10 +1534,10 @@
     <row r="5" spans="3:7">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="60" t="s">
+      <c r="E5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="60"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="3:7">
       <c r="C6" s="4" t="s">
@@ -1698,10 +1589,10 @@
         <v>3</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="3:7" ht="17">
@@ -1737,7 +1628,7 @@
     </row>
     <row r="13" spans="3:7">
       <c r="C13" s="3" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1746,10 +1637,10 @@
     <row r="14" spans="3:7">
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="60" t="s">
+      <c r="E14" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="60"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="3:7">
       <c r="C15" s="4" t="s">
@@ -1773,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="17">
@@ -1787,10 +1678,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="3:6" ht="17">
@@ -1801,10 +1692,10 @@
         <v>3</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="3:6" ht="17">
@@ -1815,10 +1706,10 @@
         <v>4</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="F19" s="20" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="3:6" ht="17" thickBot="1">
@@ -1851,7 +1742,7 @@
   </sheetPr>
   <dimension ref="D3:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1866,22 +1757,22 @@
   <sheetData>
     <row r="3" spans="4:11">
       <c r="D3" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="4:11">
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="62"/>
+      <c r="H4" s="43"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="61" t="s">
+      <c r="J4" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="62"/>
+      <c r="K4" s="43"/>
     </row>
     <row r="5" spans="4:11">
       <c r="D5" s="4" t="s">
@@ -1907,7 +1798,7 @@
     </row>
     <row r="6" spans="4:11">
       <c r="D6" s="9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="5"/>
@@ -1925,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="45">
+      <c r="G7" s="26">
         <v>33.4285979</v>
       </c>
       <c r="H7" s="13">
@@ -1947,7 +1838,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="45">
+      <c r="G8" s="26">
         <v>38.217922600000001</v>
       </c>
       <c r="H8" s="13">
@@ -1969,7 +1860,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="45">
+      <c r="G9" s="26">
         <v>16.814839500000001</v>
       </c>
       <c r="H9" s="13">
@@ -1977,7 +1868,7 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="6" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>23</v>
@@ -1991,7 +1882,7 @@
         <v>4</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="45">
+      <c r="G10" s="26">
         <v>51.751727700000004</v>
       </c>
       <c r="H10" s="13">
@@ -2028,36 +1919,36 @@
     <row r="12" spans="4:11">
       <c r="D12" s="4"/>
       <c r="E12" s="18" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="46">
+      <c r="G12" s="27">
         <v>30.273869399999999</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="28">
         <v>34</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="47" t="s">
-        <v>64</v>
+      <c r="I12" s="29"/>
+      <c r="J12" s="28" t="s">
+        <v>47</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="4:11">
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="4:11">
       <c r="D14" s="9" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -2075,7 +1966,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="7"/>
-      <c r="G15" s="49">
+      <c r="G15" s="30">
         <v>30.3156249</v>
       </c>
       <c r="H15" s="12">
@@ -2083,7 +1974,7 @@
       </c>
       <c r="I15" s="11"/>
       <c r="J15" s="12" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>15</v>
@@ -2097,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="7"/>
-      <c r="G16" s="49">
+      <c r="G16" s="30">
         <v>31.5819604</v>
       </c>
       <c r="H16" s="12">
@@ -2119,7 +2010,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="7"/>
-      <c r="G17" s="49">
+      <c r="G17" s="30">
         <v>10.339890499999999</v>
       </c>
       <c r="H17" s="12">
@@ -2141,7 +2032,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="49">
+      <c r="G18" s="30">
         <v>39.643050700000003</v>
       </c>
       <c r="H18" s="12">
@@ -2161,14 +2052,14 @@
         <v>11</v>
       </c>
       <c r="F19" s="7"/>
-      <c r="G19" s="44">
+      <c r="G19" s="25">
         <v>2273028</v>
       </c>
-      <c r="H19" s="44">
+      <c r="H19" s="25">
         <v>1338828</v>
       </c>
       <c r="I19" s="11"/>
-      <c r="J19" s="44">
+      <c r="J19" s="25">
         <v>2273028</v>
       </c>
       <c r="K19" s="10">
@@ -2178,43 +2069,43 @@
     <row r="20" spans="4:14">
       <c r="D20" s="6"/>
       <c r="E20" s="18" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F20" s="7"/>
-      <c r="G20" s="44">
+      <c r="G20" s="25">
         <v>27.467645399999999</v>
       </c>
-      <c r="H20" s="44">
+      <c r="H20" s="25">
         <v>30</v>
       </c>
       <c r="I20" s="11"/>
-      <c r="J20" s="44" t="s">
-        <v>65</v>
+      <c r="J20" s="25" t="s">
+        <v>48</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" s="82"/>
+        <v>44</v>
+      </c>
+      <c r="M20" s="61"/>
     </row>
     <row r="21" spans="4:14">
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
       <c r="I21" s="11"/>
-      <c r="J21" s="44"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="10"/>
     </row>
     <row r="22" spans="4:14">
       <c r="D22" s="9" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="11"/>
       <c r="K22" s="7"/>
     </row>
@@ -2226,14 +2117,14 @@
         <v>1</v>
       </c>
       <c r="F23" s="7"/>
-      <c r="G23" s="49">
+      <c r="G23" s="30">
         <v>90.223282499999996</v>
       </c>
       <c r="H23" s="12">
         <v>87</v>
       </c>
       <c r="I23" s="12"/>
-      <c r="J23" s="50" t="s">
+      <c r="J23" s="31" t="s">
         <v>7</v>
       </c>
       <c r="K23" s="12" t="s">
@@ -2248,14 +2139,14 @@
         <v>2</v>
       </c>
       <c r="F24" s="7"/>
-      <c r="G24" s="49">
+      <c r="G24" s="30">
         <v>103.75733289999999</v>
       </c>
       <c r="H24" s="12">
         <v>97</v>
       </c>
       <c r="I24" s="12"/>
-      <c r="J24" s="50" t="s">
+      <c r="J24" s="31" t="s">
         <v>8</v>
       </c>
       <c r="K24" s="12" t="s">
@@ -2270,14 +2161,14 @@
         <v>3</v>
       </c>
       <c r="F25" s="7"/>
-      <c r="G25" s="49">
+      <c r="G25" s="30">
         <v>72.753131999999994</v>
       </c>
       <c r="H25" s="12">
         <v>67</v>
       </c>
       <c r="I25" s="12"/>
-      <c r="J25" s="50" t="s">
+      <c r="J25" s="31" t="s">
         <v>9</v>
       </c>
       <c r="K25" s="12" t="s">
@@ -2292,14 +2183,14 @@
         <v>4</v>
       </c>
       <c r="F26" s="7"/>
-      <c r="G26" s="49">
+      <c r="G26" s="30">
         <v>153.68025689999999</v>
       </c>
       <c r="H26" s="12">
         <v>143</v>
       </c>
       <c r="I26" s="12"/>
-      <c r="J26" s="50" t="s">
+      <c r="J26" s="31" t="s">
         <v>10</v>
       </c>
       <c r="K26" s="12" t="s">
@@ -2312,14 +2203,14 @@
         <v>11</v>
       </c>
       <c r="F27" s="7"/>
-      <c r="G27" s="44">
+      <c r="G27" s="25">
         <v>40038</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="25">
         <v>26039</v>
       </c>
-      <c r="I27" s="44"/>
-      <c r="J27" s="51">
+      <c r="I27" s="25"/>
+      <c r="J27" s="32">
         <v>40038</v>
       </c>
       <c r="K27" s="10">
@@ -2329,23 +2220,23 @@
     <row r="28" spans="4:14">
       <c r="D28" s="7"/>
       <c r="E28" s="18" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F28" s="7"/>
-      <c r="G28" s="49">
+      <c r="G28" s="30">
         <v>61.128377999999998</v>
       </c>
       <c r="H28" s="12">
         <v>60</v>
       </c>
       <c r="I28" s="11"/>
-      <c r="J28" s="47" t="s">
-        <v>69</v>
+      <c r="J28" s="28" t="s">
+        <v>52</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="82"/>
+        <v>45</v>
+      </c>
+      <c r="N28" s="61"/>
     </row>
     <row r="29" spans="4:14">
       <c r="D29" s="7"/>
@@ -2354,19 +2245,19 @@
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
-      <c r="J29" s="52"/>
+      <c r="J29" s="33"/>
       <c r="K29" s="7"/>
     </row>
     <row r="30" spans="4:14">
       <c r="D30" s="9" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
-      <c r="J30" s="52"/>
+      <c r="J30" s="33"/>
       <c r="K30" s="7"/>
     </row>
     <row r="31" spans="4:14">
@@ -2377,18 +2268,18 @@
         <v>1</v>
       </c>
       <c r="F31" s="7"/>
-      <c r="G31" s="53">
+      <c r="G31" s="34">
         <v>74.190619400000003</v>
       </c>
       <c r="H31" s="12">
         <v>83</v>
       </c>
       <c r="I31" s="11"/>
-      <c r="J31" s="54" t="s">
-        <v>70</v>
+      <c r="J31" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="4:14">
@@ -2399,18 +2290,18 @@
         <v>2</v>
       </c>
       <c r="F32" s="7"/>
-      <c r="G32" s="53">
+      <c r="G32" s="34">
         <v>143.9839494</v>
       </c>
       <c r="H32" s="12">
         <v>160</v>
       </c>
       <c r="I32" s="11"/>
-      <c r="J32" s="54" t="s">
-        <v>71</v>
+      <c r="J32" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="4:15">
@@ -2421,20 +2312,20 @@
         <v>3</v>
       </c>
       <c r="F33" s="7"/>
-      <c r="G33" s="53">
+      <c r="G33" s="34">
         <v>122.73724420000001</v>
       </c>
       <c r="H33" s="12">
         <v>133</v>
       </c>
       <c r="I33" s="11"/>
-      <c r="J33" s="54" t="s">
-        <v>72</v>
+      <c r="J33" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="O33" s="82"/>
+        <v>41</v>
+      </c>
+      <c r="O33" s="61"/>
     </row>
     <row r="34" spans="4:15">
       <c r="D34" s="6">
@@ -2444,77 +2335,77 @@
         <v>4</v>
       </c>
       <c r="F34" s="7"/>
-      <c r="G34" s="53">
+      <c r="G34" s="34">
         <v>250.7462218</v>
       </c>
       <c r="H34" s="12">
         <v>268</v>
       </c>
       <c r="I34" s="11"/>
-      <c r="J34" s="54" t="s">
-        <v>73</v>
+      <c r="J34" s="35" t="s">
+        <v>56</v>
       </c>
       <c r="K34" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="4:15">
       <c r="E35" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="55">
+      <c r="G35" s="36">
         <v>117804</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="25">
         <v>120724</v>
       </c>
-      <c r="I35" s="56"/>
-      <c r="J35" s="55">
+      <c r="I35" s="37"/>
+      <c r="J35" s="36">
         <v>117804</v>
       </c>
-      <c r="K35" s="44">
+      <c r="K35" s="25">
         <v>120724</v>
       </c>
     </row>
     <row r="36" spans="4:15" ht="17" thickBot="1">
       <c r="D36" s="17"/>
       <c r="E36" s="18" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F36" s="17"/>
-      <c r="G36" s="57">
+      <c r="G36" s="38">
         <v>73.933448799999994</v>
       </c>
       <c r="H36" s="12">
         <v>74</v>
       </c>
-      <c r="I36" s="58"/>
-      <c r="J36" s="59" t="s">
-        <v>66</v>
+      <c r="I36" s="39"/>
+      <c r="J36" s="40" t="s">
+        <v>49</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="4:15">
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
-      <c r="K37" s="43"/>
-      <c r="M37" s="82"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="M37" s="61"/>
     </row>
     <row r="38" spans="4:15">
-      <c r="M38" s="82"/>
+      <c r="M38" s="61"/>
     </row>
     <row r="42" spans="4:15">
-      <c r="M42" s="82"/>
+      <c r="M42" s="61"/>
     </row>
     <row r="43" spans="4:15">
-      <c r="M43" s="82"/>
+      <c r="M43" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2530,251 +2421,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88588C20-12ED-3B49-B288-26EECA604FF5}">
   <dimension ref="E7:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="5" max="5" width="30.33203125" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="5:6" ht="33" customHeight="1" thickBot="1">
-      <c r="E7" s="100" t="s">
-        <v>152</v>
-      </c>
-      <c r="F7" s="100"/>
+      <c r="E7" s="79" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="79"/>
     </row>
     <row r="8" spans="5:6">
-      <c r="E8" s="99" t="s">
-        <v>156</v>
-      </c>
-      <c r="F8" s="99"/>
+      <c r="E8" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="78"/>
     </row>
     <row r="9" spans="5:6" ht="34">
-      <c r="E9" s="97"/>
-      <c r="F9" s="98" t="s">
-        <v>154</v>
+      <c r="E9" s="76"/>
+      <c r="F9" s="77" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="5:6">
       <c r="E10" s="1" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="5:6">
-      <c r="E11" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="66" t="s">
-        <v>123</v>
+      <c r="E11" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="5:6">
-      <c r="E12" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="F12" s="66" t="s">
-        <v>124</v>
+      <c r="E12" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="5:6">
-      <c r="E13" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="F13" s="66" t="s">
-        <v>125</v>
+      <c r="E13" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="5:6">
-      <c r="E14" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="66" t="s">
-        <v>126</v>
+      <c r="E14" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="45" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="5:6">
-      <c r="E15" s="92" t="s">
-        <v>99</v>
-      </c>
-      <c r="F15" s="66"/>
+      <c r="E15" s="71" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="45"/>
     </row>
     <row r="16" spans="5:6" ht="19">
-      <c r="E16" s="95" t="s">
-        <v>131</v>
+      <c r="E16" s="74" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="5:6" ht="19">
-      <c r="E17" s="93" t="s">
-        <v>133</v>
-      </c>
-      <c r="F17" s="93"/>
+      <c r="E17" s="72" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="72"/>
     </row>
     <row r="19" spans="5:6">
-      <c r="E19" s="99" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="99"/>
-    </row>
-    <row r="20" spans="5:6" ht="34">
-      <c r="E20" s="97"/>
-      <c r="F20" s="98" t="s">
-        <v>153</v>
+      <c r="E19" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="78"/>
+    </row>
+    <row r="20" spans="5:6" ht="51">
+      <c r="E20" s="76"/>
+      <c r="F20" s="77" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="5:6">
       <c r="E21" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6">
+      <c r="E22" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6">
+      <c r="E23" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6">
+      <c r="E24" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6">
+      <c r="E25" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" ht="19">
+      <c r="E26" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="F26" s="45"/>
+    </row>
+    <row r="27" spans="5:6" ht="19">
+      <c r="E27" s="72" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" s="72"/>
+    </row>
+    <row r="28" spans="5:6">
+      <c r="E28" s="70"/>
+    </row>
+    <row r="29" spans="5:6">
+      <c r="E29" s="63" t="s">
+        <v>111</v>
+      </c>
+      <c r="F29" s="63"/>
+    </row>
+    <row r="30" spans="5:6">
+      <c r="E30" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F30" s="69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6">
+      <c r="E31" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" s="56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6">
+      <c r="E32" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F32" s="56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11">
+      <c r="E33" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="56" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" ht="19">
+      <c r="E34" s="73" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="5:6">
-      <c r="E22" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="F22" s="66" t="s">
+      <c r="F34" s="56"/>
+    </row>
+    <row r="35" spans="5:11" ht="19">
+      <c r="E35" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="72"/>
+    </row>
+    <row r="37" spans="5:11">
+      <c r="E37" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="63"/>
+    </row>
+    <row r="38" spans="5:11">
+      <c r="E38" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11">
+      <c r="E39" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11">
+      <c r="E40" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" ht="17">
+      <c r="E41" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="K41" s="68"/>
+    </row>
+    <row r="42" spans="5:11" ht="19">
+      <c r="E42" s="73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" ht="20" thickBot="1">
+      <c r="E43" s="75" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="23" spans="5:6">
-      <c r="E23" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="F23" s="66" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="5:6">
-      <c r="E24" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="66" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="5:6">
-      <c r="E25" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="66" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="5:6" ht="19">
-      <c r="E26" s="94" t="s">
-        <v>138</v>
-      </c>
-      <c r="F26" s="66"/>
-    </row>
-    <row r="27" spans="5:6" ht="19">
-      <c r="E27" s="93" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27" s="93"/>
-    </row>
-    <row r="28" spans="5:6">
-      <c r="E28" s="91"/>
-    </row>
-    <row r="29" spans="5:6">
-      <c r="E29" s="84" t="s">
-        <v>128</v>
-      </c>
-      <c r="F29" s="84"/>
-    </row>
-    <row r="30" spans="5:6">
-      <c r="E30" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="F30" s="90" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="5:6">
-      <c r="E31" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="F31" s="77" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="5:6">
-      <c r="E32" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="F32" s="77" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="5:11">
-      <c r="E33" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="77" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="5:11" ht="19">
-      <c r="E34" s="94" t="s">
-        <v>144</v>
-      </c>
-      <c r="F34" s="77"/>
-    </row>
-    <row r="35" spans="5:11" ht="19">
-      <c r="E35" s="93" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="93"/>
-    </row>
-    <row r="37" spans="5:11">
-      <c r="E37" s="84" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="84"/>
-    </row>
-    <row r="38" spans="5:11">
-      <c r="E38" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="F38" s="66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="5:11">
-      <c r="E39" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="F39" s="66" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="5:11">
-      <c r="E40" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="F40" s="66" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="5:11" ht="17">
-      <c r="E41" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="F41" s="83" t="s">
-        <v>149</v>
-      </c>
-      <c r="K41" s="89"/>
-    </row>
-    <row r="42" spans="5:11" ht="19">
-      <c r="E42" s="94" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="5:11" ht="20" thickBot="1">
-      <c r="E43" s="96" t="s">
-        <v>151</v>
-      </c>
-      <c r="F43" s="96"/>
+      <c r="F43" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2815,205 +2706,205 @@
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="3:12" ht="17" thickBot="1">
-      <c r="C4" s="75" t="s">
-        <v>132</v>
-      </c>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
+      <c r="C4" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="3:12">
-      <c r="C5" s="72"/>
-      <c r="D5" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="76" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
     </row>
     <row r="6" spans="3:12" ht="51" customHeight="1">
       <c r="C6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="48"/>
+      <c r="I6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" ht="17">
+      <c r="C7" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="50"/>
+      <c r="I7" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" s="45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="17">
+      <c r="C8" s="58" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" s="60" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="L8" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" ht="17">
+      <c r="C9" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="G9" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="L9" s="45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" ht="17">
+      <c r="C10" s="58" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="G10" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="50"/>
+      <c r="I10" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="K10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="G6" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="69"/>
-      <c r="I6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J6" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="K6" s="69" t="s">
-        <v>113</v>
-      </c>
-      <c r="L6" s="69" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" ht="17">
-      <c r="C7" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="71" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="70" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="71" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="71"/>
-      <c r="I7" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="81" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="L7" s="66" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" ht="17">
-      <c r="C8" s="79" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="71" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="66" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="71"/>
-      <c r="I8" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="K8" s="66" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8" s="66" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="3:12" ht="17">
-      <c r="C9" s="79" t="s">
-        <v>98</v>
-      </c>
-      <c r="D9" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="71" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="78" t="s">
-        <v>109</v>
-      </c>
-      <c r="G9" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="71"/>
-      <c r="I9" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="81" t="s">
-        <v>77</v>
-      </c>
-      <c r="K9" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="L9" s="66" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" ht="17">
-      <c r="C10" s="79" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="G10" s="71" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="71"/>
-      <c r="I10" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" s="66" t="s">
-        <v>112</v>
-      </c>
-      <c r="L10" s="66" t="s">
-        <v>103</v>
+      <c r="L10" s="45" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="3:12" ht="17" thickBot="1">
-      <c r="C11" s="80" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="67">
+      <c r="C11" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="46">
         <v>2430870</v>
       </c>
-      <c r="E11" s="67"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="67">
+      <c r="E11" s="46"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="46">
         <v>1485591</v>
       </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
     </row>
     <row r="12" spans="3:12">
-      <c r="L12" s="66"/>
+      <c r="L12" s="45"/>
     </row>
     <row r="15" spans="3:12">
       <c r="D15" s="4"/>
@@ -3036,8 +2927,8 @@
       <c r="E19" s="20"/>
     </row>
     <row r="20" spans="4:5">
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3057,7 +2948,7 @@
   <dimension ref="E6:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E10"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3066,483 +2957,31 @@
   </cols>
   <sheetData>
     <row r="6" spans="5:5" ht="17" thickBot="1">
-      <c r="E6" s="85" t="s">
-        <v>122</v>
+      <c r="E6" s="64" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="5:5" ht="90">
-      <c r="E7" s="87" t="s">
-        <v>118</v>
+      <c r="E7" s="66" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="5:5" ht="75">
-      <c r="E8" s="88" t="s">
-        <v>119</v>
+      <c r="E8" s="67" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="5:5" ht="122">
-      <c r="E9" s="88" t="s">
-        <v>120</v>
+      <c r="E9" s="67" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="5:5" ht="132" customHeight="1" thickBot="1">
-      <c r="E10" s="86" t="s">
-        <v>121</v>
+      <c r="E10" s="65" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:G24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="27.6640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" style="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="27"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="28"/>
-      <c r="B2" s="63" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="64" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="63"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="32">
-        <v>332573</v>
-      </c>
-      <c r="C4" s="24">
-        <f>B4/2430870</f>
-        <v>0.13681233467853074</v>
-      </c>
-      <c r="D4" s="33">
-        <v>87078</v>
-      </c>
-      <c r="E4" s="39">
-        <f>D4/2430870</f>
-        <v>3.582174283281294E-2</v>
-      </c>
-      <c r="F4" s="34">
-        <v>47521</v>
-      </c>
-      <c r="G4" s="24">
-        <f>F4/2430870</f>
-        <v>1.9548968064931484E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="32">
-        <v>396702</v>
-      </c>
-      <c r="C5" s="24">
-        <f t="shared" ref="C5:C8" si="0">B5/2430870</f>
-        <v>0.16319342457638622</v>
-      </c>
-      <c r="D5" s="33">
-        <v>140822</v>
-      </c>
-      <c r="E5" s="39">
-        <f t="shared" ref="E5:E8" si="1">D5/2430870</f>
-        <v>5.7930699708334879E-2</v>
-      </c>
-      <c r="F5" s="34">
-        <v>86977</v>
-      </c>
-      <c r="G5" s="24">
-        <f t="shared" ref="G5:G8" si="2">F5/2430870</f>
-        <v>3.578019392234056E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="32">
-        <v>180969</v>
-      </c>
-      <c r="C6" s="24">
-        <f t="shared" si="0"/>
-        <v>7.4446185933431247E-2</v>
-      </c>
-      <c r="D6" s="33">
-        <v>86407</v>
-      </c>
-      <c r="E6" s="39">
-        <f t="shared" si="1"/>
-        <v>3.554570997214989E-2</v>
-      </c>
-      <c r="F6" s="34">
-        <v>59624</v>
-      </c>
-      <c r="G6" s="24">
-        <f t="shared" si="2"/>
-        <v>2.4527843940646766E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="32">
-        <v>593099</v>
-      </c>
-      <c r="C7" s="24">
-        <f t="shared" si="0"/>
-        <v>0.24398630942831168</v>
-      </c>
-      <c r="D7" s="33">
-        <v>249471</v>
-      </c>
-      <c r="E7" s="39">
-        <f t="shared" si="1"/>
-        <v>0.10262622024213554</v>
-      </c>
-      <c r="F7" s="34">
-        <v>160151</v>
-      </c>
-      <c r="G7" s="24">
-        <f t="shared" si="2"/>
-        <v>6.5882173871905939E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="36">
-        <v>956043</v>
-      </c>
-      <c r="C8" s="25">
-        <f t="shared" si="0"/>
-        <v>0.39329252489849315</v>
-      </c>
-      <c r="D8" s="37">
-        <v>574448</v>
-      </c>
-      <c r="E8" s="40">
-        <f t="shared" si="1"/>
-        <v>0.23631374775286215</v>
-      </c>
-      <c r="F8" s="38">
-        <v>426170</v>
-      </c>
-      <c r="G8" s="25">
-        <f t="shared" si="2"/>
-        <v>0.1753158334258928</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="28"/>
-      <c r="B11" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="63"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="32">
-        <v>384161</v>
-      </c>
-      <c r="C13" s="24">
-        <f>B13/2430870</f>
-        <v>0.15803436629684023</v>
-      </c>
-      <c r="D13" s="33">
-        <v>106240</v>
-      </c>
-      <c r="E13" s="39">
-        <f>D13/2430870</f>
-        <v>4.3704517312731658E-2</v>
-      </c>
-      <c r="F13" s="34">
-        <v>54078</v>
-      </c>
-      <c r="G13" s="24">
-        <f>F13/2430870</f>
-        <v>2.2246356242826643E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="32">
-        <v>445975</v>
-      </c>
-      <c r="C14" s="24">
-        <f t="shared" ref="C14:C17" si="3">B14/2430870</f>
-        <v>0.18346312225664063</v>
-      </c>
-      <c r="D14" s="33">
-        <v>155254</v>
-      </c>
-      <c r="E14" s="39">
-        <f t="shared" ref="E14:E17" si="4">D14/2430870</f>
-        <v>6.3867668777022213E-2</v>
-      </c>
-      <c r="F14" s="34">
-        <v>91945</v>
-      </c>
-      <c r="G14" s="24">
-        <f t="shared" ref="G14:G17" si="5">F14/2430870</f>
-        <v>3.7823906667160317E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="32">
-        <v>181602</v>
-      </c>
-      <c r="C15" s="24">
-        <f t="shared" si="3"/>
-        <v>7.4706586530748256E-2</v>
-      </c>
-      <c r="D15" s="33">
-        <v>87407</v>
-      </c>
-      <c r="E15" s="39">
-        <f t="shared" si="4"/>
-        <v>3.5957085323361594E-2</v>
-      </c>
-      <c r="F15" s="34">
-        <v>60042</v>
-      </c>
-      <c r="G15" s="24">
-        <f t="shared" si="5"/>
-        <v>2.4699798837453258E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="32">
-        <v>660120</v>
-      </c>
-      <c r="C16" s="24">
-        <f t="shared" si="3"/>
-        <v>0.2715570968418714</v>
-      </c>
-      <c r="D16" s="33">
-        <v>285807</v>
-      </c>
-      <c r="E16" s="39">
-        <f t="shared" si="4"/>
-        <v>0.11757395500376408</v>
-      </c>
-      <c r="F16" s="34">
-        <v>192901</v>
-      </c>
-      <c r="G16" s="24">
-        <f t="shared" si="5"/>
-        <v>7.9354716624089314E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="36">
-        <v>1014781</v>
-      </c>
-      <c r="C17" s="25">
-        <f t="shared" si="3"/>
-        <v>0.41745589027796631</v>
-      </c>
-      <c r="D17" s="37">
-        <v>619514</v>
-      </c>
-      <c r="E17" s="40">
-        <f t="shared" si="4"/>
-        <v>0.25485278933056887</v>
-      </c>
-      <c r="F17" s="38">
-        <v>489058</v>
-      </c>
-      <c r="G17" s="25">
-        <f t="shared" si="5"/>
-        <v>0.20118640651289457</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="D19" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="42">
-        <f>(D13-D4)/D4</f>
-        <v>0.220055582351455</v>
-      </c>
-      <c r="E20" s="41">
-        <f>D13-D4</f>
-        <v>19162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="42">
-        <f t="shared" ref="D21:D24" si="6">(D14-D5)/D5</f>
-        <v>0.10248398687705046</v>
-      </c>
-      <c r="E21" s="41">
-        <f t="shared" ref="E21:E24" si="7">D14-D5</f>
-        <v>14432</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="42">
-        <f t="shared" si="6"/>
-        <v>1.157313643570544E-2</v>
-      </c>
-      <c r="E22" s="41">
-        <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="42">
-        <f t="shared" si="6"/>
-        <v>0.14565220005531704</v>
-      </c>
-      <c r="E23" s="41">
-        <f t="shared" si="7"/>
-        <v>36336</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="42">
-        <f t="shared" si="6"/>
-        <v>7.8450965100409442E-2</v>
-      </c>
-      <c r="E24" s="41">
-        <f t="shared" si="7"/>
-        <v>45066</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>